<commit_message>
not run register success to avoid error, an account existed
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/excel/UserManagementData.xlsx
+++ b/src/test/resources/testdata/excel/UserManagementData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Selenium\E-commerce_Automation_Test\src\test\resources\testdata\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFC31F2-3A1F-4EEF-B8F7-348F0B6D5512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D187F8BE-612F-46FA-9D82-B3F885099CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
   <si>
     <t>test@gmail.com</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>john119@gmail.com</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -608,7 +611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -774,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20878650-7D9D-4C38-9189-37120C4F98C9}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -847,7 +850,7 @@
         <v>45</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add timestamp when create a new account
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/excel/UserManagementData.xlsx
+++ b/src/test/resources/testdata/excel/UserManagementData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29530"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Selenium\E-commerce_Automation_Test\src\test\resources\testdata\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D187F8BE-612F-46FA-9D82-B3F885099CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D393ED-0F2F-4388-A30F-E48F864716BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
   <si>
     <t>test@gmail.com</t>
   </si>
@@ -198,9 +198,6 @@
   </si>
   <si>
     <t>john119@gmail.com</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -778,7 +775,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -850,7 +847,7 @@
         <v>45</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>59</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>